<commit_message>
address class inbalance in training data
</commit_message>
<xml_diff>
--- a/data/Ensemble_model_result.xlsx
+++ b/data/Ensemble_model_result.xlsx
@@ -1,78 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30cf01616d186177/Documents/Local Githubs/others/smart-home-device-cyberattack-detection/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_6A69D6BF8740D224469218F14F3088B35299F7E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED396C7D-8D07-4FCF-B7D4-6926C619E150}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-26670" yWindow="2910" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Balance Accuracy</t>
-  </si>
-  <si>
-    <t>f1_score</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>Gradient Boosting</t>
-  </si>
-  <si>
-    <t>Ensemble by voting</t>
-  </si>
-  <si>
-    <t>Stacked generalization</t>
-  </si>
-  <si>
-    <t>Ada Boost Classifier</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -87,101 +46,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DF0C50D-A4EB-4CB3-9843-215140A328AE}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:D7" xr:uid="{3DF0C50D-A4EB-4CB3-9843-215140A328AE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D7">
-    <sortCondition descending="1" ref="A1:A7"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B41FA70-1B84-459F-BE62-DDA9E6BD94C2}" name="Balance Accuracy"/>
-    <tableColumn id="2" xr3:uid="{BA5211CB-AB73-4C1A-9188-415C5FFF8D38}" name="f1_score"/>
-    <tableColumn id="3" xr3:uid="{A1F75866-0B37-4559-9B25-98500E7A152F}" name="name"/>
-    <tableColumn id="4" xr3:uid="{6D92391B-56AA-429C-BAE2-9620DF17FDAC}" name="time"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -468,121 +420,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Balance Accuracy</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>f1_score</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>0.9947286821705427</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9947310860481844</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>14.43069889995968</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" t="n">
+        <v>0.9942829457364341</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9942862058363643</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>27.99852309998823</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" t="n">
+        <v>0.9942829457364341</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.9942862058363643</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>5.780775999999605</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0.99323267446111252</v>
-      </c>
-      <c r="B2">
-        <v>0.99635931505598918</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>113.8852692999935</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0.99322849350952791</v>
-      </c>
-      <c r="B3">
-        <v>0.99634758270917689</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>200.76524239999711</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.99289136027411107</v>
-      </c>
-      <c r="B4">
-        <v>0.99637226667512102</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="n">
+        <v>0.9942829457364341</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9942862058363643</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Ensemble by voting</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>27.35108829999808</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9875968992248061</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9876003504952133</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Stacked generalization</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>136.4045014000149</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>233.02872809997641</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0.99223133302163413</v>
-      </c>
-      <c r="B5">
-        <v>0.99634813599025585</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>45.525249099999201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0.99000932291832688</v>
-      </c>
-      <c r="B6">
-        <v>0.99623586621041726</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>6832.4970495000016</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0.96327781476784935</v>
-      </c>
-      <c r="B7">
-        <v>0.99429267548394296</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>86.11928290000651</v>
+      <c r="B7" t="n">
+        <v>0.9942829457364341</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.9942862058363643</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ada Boost Classifier</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>37.33918349997839</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>